<commit_message>
feat (backend): implement first version of ExcelWriter
</commit_message>
<xml_diff>
--- a/python/trials/test.xlsx
+++ b/python/trials/test.xlsx
@@ -3,11 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blatt1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mySheet_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="blatt1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,15 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>Test data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>This is another test string</t>
   </si>
   <si>
-    <t>Auch nur Testdata</t>
+    <t>Zeitraum:</t>
+  </si>
+  <si>
+    <t>Summe [km]:</t>
+  </si>
+  <si>
+    <t>Kilometergeld:</t>
+  </si>
+  <si>
+    <t>start_generated</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>km-Stand</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Ziel</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>end_generated</t>
   </si>
 </sst>
 </file>
@@ -60,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Standard" xfId="0"/>
@@ -337,44 +364,63 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.787401575" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.787401575"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="E2" s="1" t="n">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>